<commit_message>
Add results and unfolding with 100 keV threshold
</commit_message>
<xml_diff>
--- a/results/Cl36/Cl36_R_30_cm_Nr_2000000000_ISO_model_det1 - Unfolded Fluence Spectrum.xlsx
+++ b/results/Cl36/Cl36_R_30_cm_Nr_2000000000_ISO_model_det1 - Unfolded Fluence Spectrum.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,40 +511,40 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>44.62300474557222</v>
+        <v>40.35273080373261</v>
       </c>
       <c r="D2" t="n">
         <v>0.0007432820064133916</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05929019675229672</v>
+        <v>0.05768901818751787</v>
       </c>
       <c r="F2" t="n">
-        <v>66.69098885741218</v>
+        <v>249.4604156738437</v>
       </c>
       <c r="G2" t="n">
-        <v>21.66556026215645</v>
+        <v>1.452772998844936</v>
       </c>
       <c r="H2" t="n">
-        <v>96.27201835020412</v>
+        <v>520.9915530125774</v>
       </c>
       <c r="I2" t="n">
-        <v>0.003332088445736481</v>
+        <v>0.004182014977651938</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001512276245994459</v>
+        <v>5.483887722717556e-06</v>
       </c>
       <c r="K2" t="n">
-        <v>0.009516832484985045</v>
+        <v>0.01208460435650103</v>
       </c>
       <c r="L2" t="n">
-        <v>0.06359817782479807</v>
+        <v>0.0866379204398133</v>
       </c>
       <c r="M2" t="n">
-        <v>0.02497462592067068</v>
+        <v>0.0002766858027195116</v>
       </c>
       <c r="N2" t="n">
-        <v>0.09364396460676057</v>
+        <v>0.2002514646196779</v>
       </c>
     </row>
     <row r="3">
@@ -566,31 +566,77 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001027017502051611</v>
+        <v>0.0001726308312382031</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001105824364895113</v>
+        <v>7.030986138709599e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.002545120698201266</v>
+        <v>0.000285513147140896</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0003862823936146995</v>
+        <v>0.0001601665874816452</v>
       </c>
       <c r="J3" t="n">
-        <v>9.859233104093422e-05</v>
+        <v>6.567929002917165e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.000781802912675731</v>
+        <v>0.0002635850885777029</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0002918387392343568</v>
+        <v>0.0001788441461216513</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0001051134732595489</v>
+        <v>7.272893004767802e-05</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0005040660698903427</v>
+        <v>0.0002958506245513513</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Beta + Gamma</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>40.35273080373261</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0007432820064133916</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.05768901818751787</v>
+      </c>
+      <c r="F4" t="n">
+        <v>249.460588304675</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.452843308706323</v>
+      </c>
+      <c r="H4" t="n">
+        <v>520.9918385257246</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.004342181565133585</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7.116317775188921e-05</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.01234818944507873</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.08681676458593496</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0003494147327671897</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.2005473152442293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Cl36 and Sr90 results
</commit_message>
<xml_diff>
--- a/results/Cl36/Cl36_R_30_cm_Nr_2000000000_ISO_model_det1 - Unfolded Fluence Spectrum.xlsx
+++ b/results/Cl36/Cl36_R_30_cm_Nr_2000000000_ISO_model_det1 - Unfolded Fluence Spectrum.xlsx
@@ -520,31 +520,31 @@
         <v>0.05768901818751787</v>
       </c>
       <c r="F2" t="n">
-        <v>249.4604156738437</v>
+        <v>252.9574622683357</v>
       </c>
       <c r="G2" t="n">
-        <v>1.452772998844936</v>
+        <v>13.92717690194273</v>
       </c>
       <c r="H2" t="n">
-        <v>520.9915530125774</v>
+        <v>529.7361469707848</v>
       </c>
       <c r="I2" t="n">
-        <v>0.004182014977651938</v>
+        <v>0.004060232748994343</v>
       </c>
       <c r="J2" t="n">
-        <v>5.483887722717556e-06</v>
+        <v>1.236170850433409e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01208460435650103</v>
+        <v>0.01172832351857443</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0866379204398133</v>
+        <v>0.08717411495410761</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0002766858027195116</v>
+        <v>0.00253898034227455</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2002514646196779</v>
+        <v>0.2021594616209604</v>
       </c>
     </row>
     <row r="3">
@@ -566,31 +566,31 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001726308312382031</v>
+        <v>0.0001704117928854918</v>
       </c>
       <c r="G3" t="n">
-        <v>7.030986138709599e-05</v>
+        <v>6.625404822078588e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.000285513147140896</v>
+        <v>0.0002844103565428984</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0001601665874816452</v>
+        <v>0.0001580983872636318</v>
       </c>
       <c r="J3" t="n">
-        <v>6.567929002917165e-05</v>
+        <v>6.18853884043025e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0002635850885777029</v>
+        <v>0.0002624916828465526</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0001788441461216513</v>
+        <v>0.0001765591310859227</v>
       </c>
       <c r="M3" t="n">
-        <v>7.272893004767802e-05</v>
+        <v>6.854214567596484e-05</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0002958506245513513</v>
+        <v>0.0002947662782538867</v>
       </c>
     </row>
     <row r="4">
@@ -612,31 +612,31 @@
         <v>0.05768901818751787</v>
       </c>
       <c r="F4" t="n">
-        <v>249.460588304675</v>
+        <v>252.9576326801287</v>
       </c>
       <c r="G4" t="n">
-        <v>1.452843308706323</v>
+        <v>13.92724315599094</v>
       </c>
       <c r="H4" t="n">
-        <v>520.9918385257246</v>
+        <v>529.7364313811413</v>
       </c>
       <c r="I4" t="n">
-        <v>0.004342181565133585</v>
+        <v>0.004218331136257974</v>
       </c>
       <c r="J4" t="n">
-        <v>7.116317775188921e-05</v>
+        <v>7.424709690863659e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01234818944507873</v>
+        <v>0.01199081520142098</v>
       </c>
       <c r="L4" t="n">
-        <v>0.08681676458593496</v>
+        <v>0.08735067408519354</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0003494147327671897</v>
+        <v>0.002607522487950515</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2005473152442293</v>
+        <v>0.2024542278992143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add saved traces for re-loading and multipanel unfolding image
</commit_message>
<xml_diff>
--- a/results/Cl36/Cl36_R_30_cm_Nr_2000000000_ISO_model_det1 - Unfolded Fluence Spectrum.xlsx
+++ b/results/Cl36/Cl36_R_30_cm_Nr_2000000000_ISO_model_det1 - Unfolded Fluence Spectrum.xlsx
@@ -520,31 +520,31 @@
         <v>0.05768901818751787</v>
       </c>
       <c r="F2" t="n">
-        <v>252.9574622683357</v>
+        <v>254.5547444246441</v>
       </c>
       <c r="G2" t="n">
-        <v>13.92717690194273</v>
+        <v>7.234147380305044</v>
       </c>
       <c r="H2" t="n">
-        <v>529.7361469707848</v>
+        <v>531.5380277891086</v>
       </c>
       <c r="I2" t="n">
-        <v>0.004060232748994343</v>
+        <v>0.004243958145888689</v>
       </c>
       <c r="J2" t="n">
-        <v>1.236170850433409e-05</v>
+        <v>8.418800899923831e-06</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01172832351857443</v>
+        <v>0.01230523042169194</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08717411495410761</v>
+        <v>0.08759525201947291</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00253898034227455</v>
+        <v>0.001445239938877718</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2021594616209604</v>
+        <v>0.2022657148807029</v>
       </c>
     </row>
     <row r="3">
@@ -566,31 +566,31 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001704117928854918</v>
+        <v>0.0001712670374935746</v>
       </c>
       <c r="G3" t="n">
-        <v>6.625404822078588e-05</v>
+        <v>6.94120715404439e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0002844103565428984</v>
+        <v>0.0002830028873459724</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0001580983872636318</v>
+        <v>0.0001588883079206884</v>
       </c>
       <c r="J3" t="n">
-        <v>6.18853884043025e-05</v>
+        <v>6.483527485594224e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0002624916828465526</v>
+        <v>0.0002612346343260337</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0001765591310859227</v>
+        <v>0.0001774374972920838</v>
       </c>
       <c r="M3" t="n">
-        <v>6.854214567596484e-05</v>
+        <v>7.179525781898333e-05</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0002947662782538867</v>
+        <v>0.0002932562105693312</v>
       </c>
     </row>
     <row r="4">
@@ -612,31 +612,31 @@
         <v>0.05768901818751787</v>
       </c>
       <c r="F4" t="n">
-        <v>252.9576326801287</v>
+        <v>254.5549156916816</v>
       </c>
       <c r="G4" t="n">
-        <v>13.92724315599094</v>
+        <v>7.234216792376586</v>
       </c>
       <c r="H4" t="n">
-        <v>529.7364313811413</v>
+        <v>531.5383107919959</v>
       </c>
       <c r="I4" t="n">
-        <v>0.004218331136257974</v>
+        <v>0.004402846453809377</v>
       </c>
       <c r="J4" t="n">
-        <v>7.424709690863659e-05</v>
+        <v>7.325407575586609e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01199081520142098</v>
+        <v>0.01256646505601797</v>
       </c>
       <c r="L4" t="n">
-        <v>0.08735067408519354</v>
+        <v>0.08777268951676498</v>
       </c>
       <c r="M4" t="n">
-        <v>0.002607522487950515</v>
+        <v>0.001517035196696701</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2024542278992143</v>
+        <v>0.2025589710912722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>